<commit_message>
uploading renewed figure 5 and 6 and corresponding itermediate work
</commit_message>
<xml_diff>
--- a/Result/Figure5/mixture_coverage.xlsx
+++ b/Result/Figure5/mixture_coverage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17160"/>
+    <workbookView windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:L305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1064,7 +1064,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1086,7 +1086,7 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -1146,7 +1146,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="2">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -1174,7 +1174,7 @@
         <v>90</v>
       </c>
       <c r="B11" s="2">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>

</xml_diff>